<commit_message>
send email + filtering
</commit_message>
<xml_diff>
--- a/SteamGameFinder/Games Andreea Gherghescu.xlsx
+++ b/SteamGameFinder/Games Andreea Gherghescu.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="242">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="227">
   <x:si>
     <x:t>Counter-Strike: Global Offensive</x:t>
   </x:si>
@@ -32,26 +32,10 @@
     <x:t>Gratuit</x:t>
   </x:si>
   <x:si>
-    <x:t>Dota 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9 iul. 2013</x:t>
-  </x:si>
-  <x:si>
-    <x:t>War Thunder</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15 aug. 2013</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Euro Truck Simulator 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12 oct. 2012</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19,99€
-4,99€</x:t>
+    <x:t>cat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13,80€</x:t>
   </x:si>
   <x:si>
     <x:t>RimWorld</x:t>
@@ -63,220 +47,203 @@
     <x:t>32,99€</x:t>
   </x:si>
   <x:si>
-    <x:t>American Truck Simulator</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2 febr. 2016</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Phasmophobia</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18 sept. 2020</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11,59€</x:t>
-  </x:si>
-  <x:si>
     <x:t>Team Fortress 2</x:t>
   </x:si>
   <x:si>
     <x:t>10 oct. 2007</x:t>
   </x:si>
   <x:si>
-    <x:t>Farming Simulator 22</x:t>
-  </x:si>
-  <x:si>
-    <x:t>22 nov. 2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>29,99€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Left 4 Dead 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17 nov. 2009</x:t>
+    <x:t>cat notebook</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2 febr. 2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3,99€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Karate Cat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11 oct. 2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0,79€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pranky Cat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28 nov. 2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9,--€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wonder Cat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>În curând</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WonderCat Adventures</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11 sept. 2015</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2,39€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bad cat Sam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CAT GAME_xD83D__xDC31_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21 iun. 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Crazy Cat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21 febr. 2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2,99€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CAT SUDOKU_xD83D__xDC31_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14 oct. 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hidden Shapes - Cat Realm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16 nov. 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1,99€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mrs.Cat In Mars</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13 iul. 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ZEN CAT GAMES - BUNDLE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5,94€
+5,16€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ZEN CAT GAMES - FOR GIFT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5,94€
+4,87€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Relaxing Games for Cat Lovers</x:t>
+  </x:si>
+  <x:si>
+    <x:t>38,18€
+17,75€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Battle Cat vs Treacherous Mice</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16 apr. 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0,79€
+0,22€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PuzzlePet - Feed your cat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26 mart. 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Challenge Dream Cat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4 nov. 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cat's Puzzle /ᐠ｡ꞈ｡ᐟ\</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16 oct. 2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hidden Shapes Cat Realm - Premium Edition</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2,38€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DreamCat - Vânător de comori</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14 dec. 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Governor of Poker 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19 febr. 2016</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Free to Play</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sackboy™: A Big Adventure</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27 oct. 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>59,99€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hidden Shapes Cat Realm - Wallpapers</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0,99€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Past Within</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2 nov. 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5,99€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Left 4 Dead</x:t>
+  </x:si>
+  <x:si>
+    <x:t>18 nov. 2008</x:t>
   </x:si>
   <x:si>
     <x:t>9,75€</x:t>
   </x:si>
   <x:si>
-    <x:t>Factorio</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14 aug. 2020</x:t>
-  </x:si>
-  <x:si>
-    <x:t>30,--€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>World of Tanks</x:t>
-  </x:si>
-  <x:si>
-    <x:t>29 apr. 2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>House Flipper</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17 mai 2018</x:t>
-  </x:si>
-  <x:si>
-    <x:t>24,50€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>American Truck Simulator - Texas</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15 nov. 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17,99€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Car Mechanic Simulator 2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11 aug. 2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20,99€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Half-Life: Alyx</x:t>
-  </x:si>
-  <x:si>
-    <x:t>23 mart. 2020</x:t>
-  </x:si>
-  <x:si>
-    <x:t>58,99€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Euro Truck Simulator 2 - Iberia</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8 apr. 2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17,99€
-12,59€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Portal 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19 apr. 2011</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Euro Truck Simulator 2 - Scandinavia</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14 mai 2015</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17,99€
-5,39€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TUNIC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16 mart. 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>27,99€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DEVOUR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>28 ian. 2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3,99€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>WorldBox - God Simulator</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2 dec. 2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19,50€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Shakes and Fidget</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25 febr. 2016</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Euro Truck Simulator 2 - Road to the Black Sea</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5 dec. 2019</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Governor of Poker 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19 febr. 2016</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Free to Play</x:t>
-  </x:si>
-  <x:si>
-    <x:t>American Truck Simulator - Montana</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4 aug. 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11,99€
-10,79€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sackboy™: A Big Adventure</x:t>
-  </x:si>
-  <x:si>
-    <x:t>27 oct. 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>59,99€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Euro Truck Simulator 2 - Beyond the Baltic Sea</x:t>
-  </x:si>
-  <x:si>
-    <x:t>29 nov. 2018</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Past Within</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2 nov. 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5,99€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Witch It</x:t>
-  </x:si>
-  <x:si>
-    <x:t>22 oct. 2020</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Euro Truck Simulator 2 - Italia</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5 dec. 2017</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Euro Truck Simulator 2 - Vive la France !</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5 dec. 2016</x:t>
+    <x:t>House Flipper - Pets DLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12 mai 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14,79€</x:t>
   </x:si>
   <x:si>
     <x:t>Lost in Play</x:t>
@@ -289,140 +256,170 @@
 11,99€</x:t>
   </x:si>
   <x:si>
-    <x:t>Portal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Euro Truck Simulator 2 - Going East!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20 sept. 2013</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9,99€
-2,99€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Soundpad</x:t>
-  </x:si>
-  <x:si>
-    <x:t>30 sept. 2017</x:t>
+    <x:t>House Flipper - Luxury DLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14 oct. 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Farm Together</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11 oct. 2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19,99€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hydroneer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8 mai 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Tenants</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20 oct. 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24,50€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Age of History II</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22 nov. 2018</x:t>
   </x:si>
   <x:si>
     <x:t>4,99€</x:t>
   </x:si>
   <x:si>
-    <x:t>Farming Simulator 22 - Platinum Expansion</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14 nov. 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19,99€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Left 4 Dead</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18 nov. 2008</x:t>
-  </x:si>
-  <x:si>
-    <x:t>American Truck Simulator - Wyoming</x:t>
+    <x:t>Food Truck Simulator</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14 sept. 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>InfraSpace</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15 oct. 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Corsairs Legacy - Pirate Action RPG &amp; Sea Battles</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Steam Link</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10 nov. 2015</x:t>
+  </x:si>
+  <x:si>
+    <x:t>No Plan B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1 dec. 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DisplayFusion</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29 mart. 2013</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29,99€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Octodad: Dadliest Catch</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30 ian. 2014</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13,99€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Aquarist - construiește acvarii, crește pești, dezvoltă-ți afacerea!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8 mart. 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8,19€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Will You Snail?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9 mart. 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12,49€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Party Hard</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25 aug. 2015</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Slice of Sea</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11 nov. 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20,99€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>My Little Farmies</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27 febr. 2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Milo and the Magpies</x:t>
   </x:si>
   <x:si>
     <x:t>7 sept. 2021</x:t>
   </x:si>
   <x:si>
-    <x:t>11,99€
-8,39€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>A Dance of Fire and Ice</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25 ian. 2019</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Soul Dossier</x:t>
-  </x:si>
-  <x:si>
-    <x:t>mart. 2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Universe Sandbox</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25 aug. 2015</x:t>
-  </x:si>
-  <x:si>
-    <x:t>28,99€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>American Truck Simulator - Colorado</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12 nov. 2020</x:t>
+    <x:t>Gibbous - A Cthulhu Adventure</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7 aug. 2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19,99€
+5,99€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Workers &amp; Resources: Soviet Republic</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15 mart. 2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Paragon: The Overprime</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6 dec. 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>American Truck Simulator - Idaho</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16 iul. 2020</x:t>
   </x:si>
   <x:si>
     <x:t>11,99€
 5,99€</x:t>
   </x:si>
   <x:si>
-    <x:t>House Flipper - Pets DLC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12 mai 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14,79€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Euro Truck Simulator 2 Map Booster</x:t>
-  </x:si>
-  <x:si>
-    <x:t>99,94€
-25,44€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Keep Talking and Nobody Explodes</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8 oct. 2015</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14,99€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Black Mesa</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6 mart. 2020</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Farming Simulator 19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20 nov. 2018</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Euro Truck Simulator 2 Essentials</x:t>
-  </x:si>
-  <x:si>
-    <x:t>59,94€
-14,40€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Paragon: The Overprime</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6 dec. 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>House Flipper - Luxury DLC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14 oct. 2021</x:t>
-  </x:si>
-  <x:si>
     <x:t>Scorn</x:t>
   </x:si>
   <x:si>
@@ -432,46 +429,16 @@
     <x:t>39,99€</x:t>
   </x:si>
   <x:si>
-    <x:t>Farm Together</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11 oct. 2018</x:t>
-  </x:si>
-  <x:si>
-    <x:t>American Truck Simulator - Idaho</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16 iul. 2020</x:t>
-  </x:si>
-  <x:si>
     <x:t>Backpack Hero</x:t>
   </x:si>
   <x:si>
     <x:t>15 aug. 2022</x:t>
   </x:si>
   <x:si>
-    <x:t>13,99€</x:t>
-  </x:si>
-  <x:si>
     <x:t>Car Mechanic Simulator 2021 - Drag Racing DLC</x:t>
   </x:si>
   <x:si>
     <x:t>9 nov. 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12,49€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hydroneer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8 mai 2020</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Workers &amp; Resources: Soviet Republic</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15 mart. 2019</x:t>
   </x:si>
   <x:si>
     <x:t>American Truck Simulator - Utah</x:t>
@@ -490,6 +457,15 @@
     <x:t>30 nov. 2022</x:t>
   </x:si>
   <x:si>
+    <x:t>Paint the Town Red</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29 iul. 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19,50€</x:t>
+  </x:si>
+  <x:si>
     <x:t>Euro Truck Simulator 2 - High Power Cargo Pack</x:t>
   </x:si>
   <x:si>
@@ -500,37 +476,22 @@
 1,49€</x:t>
   </x:si>
   <x:si>
+    <x:t>American Truck Simulator - New Mexico</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9 nov. 2017</x:t>
+  </x:si>
+  <x:si>
     <x:t>House Flipper - Garden DLC</x:t>
   </x:si>
   <x:si>
     <x:t>16 mai 2019</x:t>
   </x:si>
   <x:si>
-    <x:t>American Truck Simulator - New Mexico</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9 nov. 2017</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Paint the Town Red</x:t>
-  </x:si>
-  <x:si>
-    <x:t>29 iul. 2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Element TD 2 - Tower Defense</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2 apr. 2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14,--€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Tenants</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20 oct. 2022</x:t>
+    <x:t>American Truck Simulator - Oregon</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4 oct. 2018</x:t>
   </x:si>
   <x:si>
     <x:t>American Truck Simulator - Washington</x:t>
@@ -539,16 +500,21 @@
     <x:t>11 iun. 2019</x:t>
   </x:si>
   <x:si>
-    <x:t>Kingdoms and Castles</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20 iul. 2017</x:t>
-  </x:si>
-  <x:si>
-    <x:t>American Truck Simulator - Oregon</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4 oct. 2018</x:t>
+    <x:t>WW2 Rebuilder + House Flipper</x:t>
+  </x:si>
+  <x:si>
+    <x:t>41,29€
+35,65€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Euro Truck Simulator 2 - Cabin Accessories</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30 sept. 2015</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3,99€
+1,19€</x:t>
   </x:si>
   <x:si>
     <x:t>Northwest Bundle</x:t>
@@ -558,14 +524,13 @@
 38,25€</x:t>
   </x:si>
   <x:si>
-    <x:t>Euro Truck Simulator 2 - Cabin Accessories</x:t>
-  </x:si>
-  <x:si>
-    <x:t>30 sept. 2015</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3,99€
-1,19€</x:t>
+    <x:t>Element TD 2 - Tower Defense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2 apr. 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14,--€</x:t>
   </x:si>
   <x:si>
     <x:t>Tricky Towers</x:t>
@@ -574,13 +539,7 @@
     <x:t>2 aug. 2016</x:t>
   </x:si>
   <x:si>
-    <x:t>Mindustry</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26 sept. 2019</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9,99€</x:t>
+    <x:t>14,99€</x:t>
   </x:si>
   <x:si>
     <x:t>Euro Truck Simulator 2 - Volvo Construction Equipment</x:t>
@@ -599,12 +558,24 @@
     <x:t>5 mart. 2020</x:t>
   </x:si>
   <x:si>
+    <x:t>Kingdoms and Castles</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20 iul. 2017</x:t>
+  </x:si>
+  <x:si>
     <x:t>House Flipper - HGTV DLC</x:t>
   </x:si>
   <x:si>
     <x:t>14 mai 2020</x:t>
   </x:si>
   <x:si>
+    <x:t>Euro Truck Simulator 2 - Special Transport</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13 dec. 2017</x:t>
+  </x:si>
+  <x:si>
     <x:t>MADiSON</x:t>
   </x:si>
   <x:si>
@@ -614,82 +585,82 @@
     <x:t>34,99€</x:t>
   </x:si>
   <x:si>
-    <x:t>Euro Truck Simulator 2 - Special Transport</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13 dec. 2017</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Legion TD 2 - Multiplayer Tower Defense</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1 oct. 2021</x:t>
-  </x:si>
-  <x:si>
     <x:t>War Thunder - F-5C Pack</x:t>
   </x:si>
   <x:si>
     <x:t>7 iun. 2021</x:t>
   </x:si>
   <x:si>
+    <x:t>Mindustry</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26 sept. 2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9,99€</x:t>
+  </x:si>
+  <x:si>
     <x:t>Euro Truck Simulator 2 - Heavy Cargo Pack</x:t>
   </x:si>
   <x:si>
     <x:t>12 mai 2017</x:t>
   </x:si>
   <x:si>
-    <x:t>Age of History II</x:t>
-  </x:si>
-  <x:si>
-    <x:t>22 nov. 2018</x:t>
-  </x:si>
-  <x:si>
     <x:t>War Thunder - Leopard 2A4 Pack</x:t>
   </x:si>
   <x:si>
     <x:t>15 iun. 2022</x:t>
   </x:si>
   <x:si>
+    <x:t>Euro Truck Simulator 2 - Wheel Tuning Pack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13 apr. 2016</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2,99€
+0,89€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Subsistence</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25 oct. 2016</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Southwest Bundle</x:t>
+  </x:si>
+  <x:si>
+    <x:t>70,92€
+20,71€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Townscaper</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26 aug. 2021</x:t>
+  </x:si>
+  <x:si>
     <x:t>SpeedRunners</x:t>
   </x:si>
   <x:si>
     <x:t>19 apr. 2016</x:t>
   </x:si>
   <x:si>
-    <x:t>Euro Truck Simulator 2 - Renault Trucks T Tuning Pack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25 mai 2022</x:t>
+    <x:t>DSX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24 iun. 2022</x:t>
   </x:si>
   <x:si>
     <x:t>3,99€
 3,59€</x:t>
   </x:si>
   <x:si>
-    <x:t>Euro Truck Simulator 2 - Wheel Tuning Pack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13 apr. 2016</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2,99€
-0,89€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DSX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>24 iun. 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3,99€
-3,39€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Townscaper</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26 aug. 2021</x:t>
+    <x:t>Euro Truck Simulator 2 - Renault Trucks T Tuning Pack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25 mai 2022</x:t>
   </x:si>
   <x:si>
     <x:t>War Thunder - MiG-23ML Pack</x:t>
@@ -699,19 +670,6 @@
   </x:si>
   <x:si>
     <x:t>69,99€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Southwest Bundle</x:t>
-  </x:si>
-  <x:si>
-    <x:t>70,92€
-20,71€</x:t>
-  </x:si>
-  <x:si>
-    <x:t>War Thunder - A-10A Thunderbolt (Early) Pack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25 mart. 2022</x:t>
   </x:si>
   <x:si>
     <x:t>Euro Truck Simulator 2 - FH Tuning Pack</x:t>
@@ -724,28 +682,10 @@
 2,79€</x:t>
   </x:si>
   <x:si>
-    <x:t>shapez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7 iun. 2020</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Subsistence</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25 oct. 2016</x:t>
-  </x:si>
-  <x:si>
-    <x:t>American Truck Simulator - Special Transport</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7 nov. 2018</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Farming Simulator 17</x:t>
-  </x:si>
-  <x:si>
-    <x:t>24 oct. 2016</x:t>
+    <x:t>War Thunder - A-10A Thunderbolt (Early) Pack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25 mart. 2022</x:t>
   </x:si>
   <x:si>
     <x:t>American Truck Simulator - Forest Machinery</x:t>
@@ -755,19 +695,32 @@
 2,49€</x:t>
   </x:si>
   <x:si>
-    <x:t>Food Truck Simulator</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14 sept. 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>American Truck Simulator - Wild West Paint Jobs Pack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1,99€</x:t>
+    <x:t>Texas-sized Bundle</x:t>
+  </x:si>
+  <x:si>
+    <x:t>66,92€
+30,07€</x:t>
+  </x:si>
+  <x:si>
+    <x:t>American Truck Simulator - Special Transport</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7 nov. 2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Portal Bundle</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14,62€</x:t>
   </x:si>
   <x:si>
     <x:t>American Truck Simulator - Volvo Construction Equipment</x:t>
+  </x:si>
+  <x:si>
+    <x:t>shapez</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7 iun. 2020</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1137,11 +1090,8 @@
       <x:c r="A2" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="C2" s="0" t="s">
         <x:v>4</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1152,18 +1102,18 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A4" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1185,1029 +1135,999 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A7" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A8" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A9" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A10" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="C10" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A11" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A12" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
         <x:v>29</x:v>
-      </x:c>
-      <x:c r="B12" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="C12" s="0" t="s">
-        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A13" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="B13" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A14" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
         <x:v>34</x:v>
-      </x:c>
-      <x:c r="B14" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="C14" s="0" t="s">
-        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A15" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A16" s="0" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="B16" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A17" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="B17" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A18" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="B18" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A19" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A20" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A21" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A22" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="C22" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A23" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="B23" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A24" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A25" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A26" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A27" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A28" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A29" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A30" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="C30" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A31" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A32" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="C32" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A33" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="C33" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A34" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C34" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A35" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C35" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A36" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="C36" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A37" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="C37" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A38" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A39" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="C39" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A40" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>103</x:v>
-      </x:c>
-      <x:c r="C40" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A41" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C41" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A42" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="C42" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A43" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="C43" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A44" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="C44" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A45" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="s">
+        <x:v>109</x:v>
       </x:c>
       <x:c r="C45" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A46" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="C46" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A47" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C47" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A48" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="C48" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A49" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
+        <x:v>119</x:v>
       </x:c>
       <x:c r="C49" s="0" t="s">
-        <x:v>125</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A50" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="C50" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>122</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:3">
       <x:c r="A51" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="C51" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:3">
       <x:c r="A52" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C52" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:3">
       <x:c r="A53" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C53" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:3">
       <x:c r="A54" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C54" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:3">
       <x:c r="A55" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="C55" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:3">
       <x:c r="A56" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="C56" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:3">
       <x:c r="A57" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="C57" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:3">
       <x:c r="A58" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="C58" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:3">
       <x:c r="A59" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C59" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:3">
       <x:c r="A60" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>151</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="C60" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:3">
       <x:c r="A61" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="C61" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:3">
       <x:c r="A62" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="C62" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:3">
       <x:c r="A63" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="C63" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:3">
       <x:c r="A64" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="B64" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="C64" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:3">
       <x:c r="A65" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="C65" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:3">
       <x:c r="A66" s="0" t="s">
-        <x:v>164</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="B66" s="0" t="s">
-        <x:v>165</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="C66" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="67" spans="1:3">
       <x:c r="A67" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="B67" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="C67" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="68" spans="1:3">
       <x:c r="A68" s="0" t="s">
-        <x:v>168</x:v>
-      </x:c>
-      <x:c r="B68" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="C68" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="69" spans="1:3">
       <x:c r="A69" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="B69" s="0" t="s">
-        <x:v>171</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="C69" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>160</x:v>
       </x:c>
     </x:row>
     <x:row r="70" spans="1:3">
       <x:c r="A70" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="C70" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>162</x:v>
       </x:c>
     </x:row>
     <x:row r="71" spans="1:3">
       <x:c r="A71" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="B71" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C71" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="72" spans="1:3">
       <x:c r="A72" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="B72" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="C72" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>165</x:v>
       </x:c>
     </x:row>
     <x:row r="73" spans="1:3">
       <x:c r="A73" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="B73" s="0" t="s">
-        <x:v>180</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="C73" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>168</x:v>
       </x:c>
     </x:row>
     <x:row r="74" spans="1:3">
       <x:c r="A74" s="0" t="s">
-        <x:v>182</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="B74" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="C74" s="0" t="s">
-        <x:v>184</x:v>
+        <x:v>171</x:v>
       </x:c>
     </x:row>
     <x:row r="75" spans="1:3">
       <x:c r="A75" s="0" t="s">
-        <x:v>185</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="B75" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="C75" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="1:3">
       <x:c r="A76" s="0" t="s">
-        <x:v>187</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="B76" s="0" t="s">
-        <x:v>188</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="C76" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="77" spans="1:3">
       <x:c r="A77" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="B77" s="0" t="s">
-        <x:v>190</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="C77" s="0" t="s">
-        <x:v>191</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="78" spans="1:3">
       <x:c r="A78" s="0" t="s">
-        <x:v>192</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="B78" s="0" t="s">
-        <x:v>193</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="C78" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:3">
       <x:c r="A79" s="0" t="s">
-        <x:v>194</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="B79" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="C79" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>182</x:v>
       </x:c>
     </x:row>
     <x:row r="80" spans="1:3">
       <x:c r="A80" s="0" t="s">
-        <x:v>196</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="B80" s="0" t="s">
-        <x:v>197</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="C80" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:3">
       <x:c r="A81" s="0" t="s">
-        <x:v>198</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="B81" s="0" t="s">
-        <x:v>199</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="C81" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>187</x:v>
       </x:c>
     </x:row>
     <x:row r="82" spans="1:3">
       <x:c r="A82" s="0" t="s">
-        <x:v>200</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="B82" s="0" t="s">
-        <x:v>201</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="C82" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:3">
       <x:c r="A83" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="B83" s="0" t="s">
-        <x:v>203</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="C83" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="84" spans="1:3">
       <x:c r="A84" s="0" t="s">
-        <x:v>204</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="B84" s="0" t="s">
-        <x:v>205</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="C84" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>194</x:v>
       </x:c>
     </x:row>
     <x:row r="85" spans="1:3">
       <x:c r="A85" s="0" t="s">
-        <x:v>206</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="B85" s="0" t="s">
-        <x:v>207</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="C85" s="0" t="s">
-        <x:v>208</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="86" spans="1:3">
       <x:c r="A86" s="0" t="s">
-        <x:v>209</x:v>
-      </x:c>
-      <x:c r="B86" s="0" t="s">
-        <x:v>210</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="C86" s="0" t="s">
-        <x:v>211</x:v>
+        <x:v>198</x:v>
       </x:c>
     </x:row>
     <x:row r="87" spans="1:3">
       <x:c r="A87" s="0" t="s">
-        <x:v>212</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="B87" s="0" t="s">
-        <x:v>213</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="C87" s="0" t="s">
-        <x:v>214</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="88" spans="1:3">
       <x:c r="A88" s="0" t="s">
-        <x:v>215</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="B88" s="0" t="s">
-        <x:v>216</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="C88" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="89" spans="1:3">
       <x:c r="A89" s="0" t="s">
-        <x:v>217</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="B89" s="0" t="s">
-        <x:v>218</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="C89" s="0" t="s">
-        <x:v>219</x:v>
+        <x:v>168</x:v>
       </x:c>
     </x:row>
     <x:row r="90" spans="1:3">
       <x:c r="A90" s="0" t="s">
-        <x:v>220</x:v>
+        <x:v>203</x:v>
+      </x:c>
+      <x:c r="B90" s="0" t="s">
+        <x:v>204</x:v>
       </x:c>
       <x:c r="C90" s="0" t="s">
-        <x:v>221</x:v>
+        <x:v>205</x:v>
       </x:c>
     </x:row>
     <x:row r="91" spans="1:3">
       <x:c r="A91" s="0" t="s">
-        <x:v>222</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="B91" s="0" t="s">
-        <x:v>223</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="C91" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>205</x:v>
       </x:c>
     </x:row>
     <x:row r="92" spans="1:3">
       <x:c r="A92" s="0" t="s">
-        <x:v>224</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="B92" s="0" t="s">
-        <x:v>225</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="C92" s="0" t="s">
-        <x:v>226</x:v>
+        <x:v>210</x:v>
       </x:c>
     </x:row>
     <x:row r="93" spans="1:3">
       <x:c r="A93" s="0" t="s">
-        <x:v>227</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="B93" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="C93" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>213</x:v>
       </x:c>
     </x:row>
     <x:row r="94" spans="1:3">
       <x:c r="A94" s="0" t="s">
-        <x:v>229</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="B94" s="0" t="s">
-        <x:v>230</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="C94" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="95" spans="1:3">
       <x:c r="A95" s="0" t="s">
-        <x:v>231</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="B95" s="0" t="s">
-        <x:v>232</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="C95" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>217</x:v>
       </x:c>
     </x:row>
     <x:row r="96" spans="1:3">
       <x:c r="A96" s="0" t="s">
-        <x:v>233</x:v>
-      </x:c>
-      <x:c r="B96" s="0" t="s">
-        <x:v>234</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="C96" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>219</x:v>
       </x:c>
     </x:row>
     <x:row r="97" spans="1:3">
       <x:c r="A97" s="0" t="s">
-        <x:v>235</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="B97" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="C97" s="0" t="s">
-        <x:v>236</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="98" spans="1:3">
       <x:c r="A98" s="0" t="s">
-        <x:v>237</x:v>
-      </x:c>
-      <x:c r="B98" s="0" t="s">
-        <x:v>238</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="C98" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>223</x:v>
       </x:c>
     </x:row>
     <x:row r="99" spans="1:3">
       <x:c r="A99" s="0" t="s">
-        <x:v>239</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="B99" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="C99" s="0" t="s">
-        <x:v>240</x:v>
+        <x:v>171</x:v>
       </x:c>
     </x:row>
     <x:row r="100" spans="1:3">
       <x:c r="A100" s="0" t="s">
-        <x:v>241</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="B100" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="C100" s="0" t="s">
-        <x:v>184</x:v>
+        <x:v>187</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>